<commit_message>
Shipper Contact Code Commit
</commit_message>
<xml_diff>
--- a/TestData/Carrier.xlsx
+++ b/TestData/Carrier.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Carrier Name;DOT #;MC #;Invite</t>
+  </si>
+  <si>
+    <t>Company Added Successfully</t>
   </si>
 </sst>
 </file>
@@ -127,7 +130,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -150,12 +153,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
@@ -163,6 +177,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -468,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,9 +499,11 @@
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,8 +525,17 @@
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="H1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -529,6 +556,9 @@
       </c>
       <c r="G2" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -545,7 +575,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,7 +631,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection sqref="A1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>